<commit_message>
Salabotas garumzimes visā sistēmā
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8670"/>
   </bookViews>
@@ -18,8 +13,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>Nr.</t>
   </si>
@@ -217,8 +212,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,14 +350,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,21 +659,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -689,7 +684,7 @@
     <col min="7" max="7" width="38.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -712,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -733,7 +728,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="150">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -754,7 +749,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -775,7 +770,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="195">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -796,7 +791,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="135">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -817,7 +812,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="135">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -838,7 +833,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -859,7 +854,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -878,7 +873,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -901,7 +896,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -922,7 +917,7 @@
       </c>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -943,26 +938,28 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="E13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="60">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -981,7 +978,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="90">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1000,7 +997,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -1019,134 +1016,134 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+    <row r="17" spans="1:7" ht="60">
+      <c r="A17" s="18">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="18">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" ht="90">
+      <c r="A19" s="18">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="18">
         <v>19</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="D26" s="3"/>
       <c r="E26" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="1"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="1"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="1"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="1"/>
       <c r="D31" s="3"/>
     </row>

</xml_diff>

<commit_message>
15 un 18 kļūda, labota
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>Nr.</t>
   </si>
@@ -207,6 +207,12 @@
   <si>
     <t>1. Pēc meklēšanas pielikt izvēlni "check-all" jeb atzīmēt visus meklēšanas rezultātus
 2. Veidojot mācību grupu, pēc lauka "Izvēlieties mācību kursu", pievienot jaunu teksta ievades lauku "Ievadiet mācību grupas nosaukumu", jāveic papildinājumi arī datubāzē</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Vēl jāizlabo trešais punkts</t>
   </si>
 </sst>
 </file>
@@ -305,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,12 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -358,6 +358,18 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -669,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -780,7 +792,7 @@
       <c r="C5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -915,7 +927,7 @@
       <c r="F11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="10">
@@ -942,7 +954,7 @@
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -998,102 +1010,108 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="30">
-      <c r="A16" s="14">
+      <c r="A16" s="21">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="60">
+      <c r="A17" s="16">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="60">
-      <c r="A17" s="18">
-        <v>16</v>
-      </c>
-      <c r="B17" s="18" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="18" t="s">
+      <c r="C18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" ht="30">
-      <c r="A18" s="18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="18" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" ht="90">
+      <c r="A19" s="19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" ht="90">
-      <c r="A19" s="18">
-        <v>18</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="18">
+      <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
Dažādi labojumi no labojumu arhiva
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -213,6 +213,14 @@
   </si>
   <si>
     <t>Vēl jāizlabo trešais punkts</t>
+  </si>
+  <si>
+    <t>searchRoom.php
+searchCourse.php
+searchPerson.php</t>
+  </si>
+  <si>
+    <t>1.Jāatveras pareizajām profila lapām</t>
   </si>
 </sst>
 </file>
@@ -311,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,6 +377,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -671,7 +694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -681,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="A18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,23 +1054,25 @@
       <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" ht="60">
-      <c r="A17" s="16">
+      <c r="A17" s="24">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="E17" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="A18" s="16">
@@ -1091,23 +1116,33 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="16">
+    <row r="20" spans="1:7" ht="45">
+      <c r="A20" s="24">
         <v>19</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="B20" s="25">
+        <v>42338</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="16">
         <v>20</v>
       </c>
       <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="17"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>

</xml_diff>

<commit_message>
Atšķirīga lapa pēc login v1.0
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -319,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -392,6 +392,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -694,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,7 +711,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,23 +896,25 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="12">
+      <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="E9" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="30">
       <c r="A10" s="10">

</xml_diff>

<commit_message>
Papildināts labojumu excel fails
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\MCVS\MCVS\Dok\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8670"/>
   </bookViews>
@@ -13,8 +18,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>Nr.</t>
   </si>
@@ -220,14 +225,32 @@
 searchPerson.php</t>
   </si>
   <si>
-    <t>1.Jāatveras pareizajām profila lapām</t>
+    <t>30.11.2015.</t>
+  </si>
+  <si>
+    <t>1. Jāatveras pareizajām profila lapām</t>
+  </si>
+  <si>
+    <t>02.12.2015.</t>
+  </si>
+  <si>
+    <t>1. Ja lietotājs nav pievienojis porfila bildi, nepieciešams attēlot noklusējuma bildi</t>
+  </si>
+  <si>
+    <t>user-page.php
+searchRoom.php
+searchCourse.php
+searchPerson.php</t>
+  </si>
+  <si>
+    <t>1. Lauku "Lietotāja loma" vajag virs laukiem "apgūtie kursi, iegūtie diplomi, iegūtie sertifikāti, pasniedzamie kursi"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -378,9 +401,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -700,21 +720,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -725,7 +745,7 @@
     <col min="7" max="7" width="38.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -748,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -769,7 +789,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="150">
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -790,7 +810,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -811,7 +831,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="195">
+    <row r="5" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -832,7 +852,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="135">
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -853,7 +873,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="135">
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -874,7 +894,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -895,28 +915,28 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="28">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
         <v>8</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:7" ht="30">
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -939,7 +959,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -960,7 +980,7 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -981,7 +1001,7 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1002,7 +1022,7 @@
       </c>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="60">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1021,7 +1041,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="90">
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1040,7 +1060,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -1061,28 +1081,28 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="60">
-      <c r="A17" s="24">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="24" t="s">
+      <c r="E17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" spans="1:7" ht="30">
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>17</v>
       </c>
@@ -1101,7 +1121,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -1124,89 +1144,116 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45">
-      <c r="A20" s="24">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
         <v>19</v>
       </c>
-      <c r="B20" s="25">
-        <v>42338</v>
-      </c>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="D20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="E25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="E26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="E27" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Atjaunots labojumu excel dok.
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -728,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,40 +1204,47 @@
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="16">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="5" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="4" t="s">
-        <v>7</v>
+      <c r="E25" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="7" t="s">
-        <v>8</v>
+      <c r="E26" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="6" t="s">
-        <v>4</v>
+      <c r="E27" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="D28" s="3"/>
+      <c r="E28" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -1254,6 +1261,10 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Papildināts kļūdu un labojumu excelis
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\MCVS\MCVS\Dok\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8670"/>
   </bookViews>
@@ -13,8 +18,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
   <si>
     <t>Nr.</t>
   </si>
@@ -241,14 +246,29 @@
     <t>1. Lauku "Lietotāja loma" vajag virs laukiem "apgūtie kursi, iegūtie diplomi, iegūtie sertifikāti, pasniedzamie kursi"</t>
   </si>
   <si>
-    <t>Nestrādā poga pievienot</t>
+    <t>12.12.2015.</t>
+  </si>
+  <si>
+    <t>08.12.2015.</t>
+  </si>
+  <si>
+    <t>user-pageForUser.php</t>
+  </si>
+  <si>
+    <t>1. Nestrādā poga "Pievienot"</t>
+  </si>
+  <si>
+    <t>1. Ielogojoties ar lietotāju, kura tiesības atbilst pasniedzēja līmenim parādās lapa profile.php, kurā attēlots nenostilots lauks "Mācību GRUPU PLĀNOŠANA"</t>
+  </si>
+  <si>
+    <t>1. Lauks "Nav ievadīts lietotājvārds un / vai parole!" jānostilo, lai tas ir zem pogas "Ienākt sistēmā"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,32 +735,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -763,7 +783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -784,7 +804,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="150">
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -805,7 +825,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -826,7 +846,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="195">
+    <row r="5" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -847,7 +867,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="135">
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -868,7 +888,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="135">
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -889,7 +909,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -910,7 +930,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -931,7 +951,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -954,7 +974,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -975,7 +995,7 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -996,7 +1016,7 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1017,7 +1037,7 @@
       </c>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="60">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1036,7 +1056,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="90">
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1055,7 +1075,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -1076,7 +1096,7 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="60">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -1097,7 +1117,7 @@
       </c>
       <c r="G17" s="23"/>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -1118,7 +1138,7 @@
       </c>
       <c r="G18" s="23"/>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -1141,7 +1161,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -1162,7 +1182,7 @@
       </c>
       <c r="G20" s="23"/>
     </row>
-    <row r="21" spans="1:7" ht="45">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -1183,7 +1203,7 @@
       </c>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" ht="60">
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -1204,76 +1224,179 @@
       </c>
       <c r="G22" s="23"/>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="16">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
         <v>22</v>
       </c>
-      <c r="B23" s="27">
-        <v>42346</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="C24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="1"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="1"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="1"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="1"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>24</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>25</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="D33" s="3"/>
+      <c r="E33" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="D40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mazi labojumi no kļūdu labojumu dienasgrāmatas
</commit_message>
<xml_diff>
--- a/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
+++ b/Dok/Labojumu_un_papildinajumu_arhivs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
   <si>
     <t>Nr.</t>
   </si>
@@ -262,10 +262,6 @@
     <t>03.01.2016.</t>
   </si>
   <si>
-    <t>1. Jāpieliek lauks "Auditorijas adrese"
-2. Vārdā "tāfele" drukas kļūda</t>
-  </si>
-  <si>
     <t>searchCourse.php</t>
   </si>
   <si>
@@ -278,6 +274,9 @@
   </si>
   <si>
     <t>Daļa vairs nav aktuāla, bet viss pārejais ir izlabots</t>
+  </si>
+  <si>
+    <t>1. Jāpieliek lauks "Auditorijas adrese"</t>
   </si>
 </sst>
 </file>
@@ -745,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -755,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,7 +1087,7 @@
         <v>38</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30">
@@ -1281,23 +1280,25 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="60">
-      <c r="A25" s="14">
+      <c r="A25" s="21">
         <v>24</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="E25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" ht="45">
       <c r="A26" s="14">
@@ -1318,7 +1319,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>6</v>
@@ -1338,42 +1339,46 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" ht="105">
-      <c r="A28" s="14">
+      <c r="A28" s="21">
         <v>27</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="E28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="21">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="14">
-        <v>28</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="E29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="14">

</xml_diff>